<commit_message>
Se actualiza USM con releases
</commit_message>
<xml_diff>
--- a/USM-Grupo 8.xlsx
+++ b/USM-Grupo 8.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joaquin\Desktop\UNI EXACTAS\TUDAI\2 1 Intr. Metodologia de Software\GIT TPE Metodologías Grupo 8\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="USM " sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>USER</t>
   </si>
@@ -106,13 +114,10 @@
     <t>Como secretaria quiero cargar días y horarios disponibles del médico, para que los pacientes tengan turnos disponibles. (TF-6)</t>
   </si>
   <si>
-    <t>Como secretaria quiero cargar turnos para cada médico con el que trabajo para los casos en que el paciente no pueda cargárselo. (TF-7)</t>
-  </si>
-  <si>
     <t>Como médico quiero acceder a la aplicación ingresando nombre de usuario y contraseña para así poder operar en la plataforma de forma segura. (TF-16)</t>
   </si>
   <si>
-    <t>Como médico quiero filtrar las listas de turnos venideros para así poder organizar mi agenda. (TF-17)</t>
+    <t>Como médico quiero ver la lista de turnos venideros para así poder organizar mi agenda. (TF-33)</t>
   </si>
   <si>
     <t>Como responsable de la institución médica quiero crear usuarios para secretarias y médicos de esa institución. (TF-25)</t>
@@ -127,74 +132,91 @@
     <t>Como paciente quiero ver mis próximos turnos para recordar los turnos solicitados. (TF-29)</t>
   </si>
   <si>
+    <t>Como paciente quiero visualizar los días y horarios del médico que seleccioné para poder elegir el turno que más me convenga. (TF-23)</t>
+  </si>
+  <si>
+    <t>fin MVP / fin Release 1</t>
+  </si>
+  <si>
+    <t>Como paciente quiero indicar un rango de fechas para visualizar los turnos y/o indicar el turno de preferencia (TF-24)</t>
+  </si>
+  <si>
     <t>Como secretaria quiero filtrar la lista de los turnos venideros para organizar la agenda de los médicos. (TF-14)</t>
   </si>
   <si>
     <t>Como secretaria quiero definir para la franja horaria de un día y médico determinado la duración de cada turno, para agilizar la carga de turnos disponibles. (TF-8)</t>
   </si>
   <si>
+    <t>Como secretaria quiero cargar turnos a cada médico con el que trabajo para los casos en que el paciente no pueda cargárselo. (TF-7)</t>
+  </si>
+  <si>
+    <t>Como médico quiero filtrar la lista de turnos venideros para así poder organizar mi agenda.. (TF-17)</t>
+  </si>
+  <si>
+    <t>Como paciente quiero visualizar los turnos disponibles de acuerdo al filtro indicado para poder sacar un nuevo turno. (TF-1)</t>
+  </si>
+  <si>
+    <t>Como secretaria quiero guardar el filtro de la lista de forma periódica y que se imprima la lista automáticamente para así optimizar el tiempo de consultas reiterativas. (TF-15)</t>
+  </si>
+  <si>
     <t>Como secretaria quiero cancelar turnos para cuando a un médico le surge una urgencia. (TF-9)</t>
   </si>
   <si>
-    <t>Como paciente quiero visualizar los días y horarios del médico que seleccioné para poder elegir el turno que más me convenga. (TF-23)</t>
-  </si>
-  <si>
     <t>Como paciente quiero visualizar el detalle del turno registrado en la aplicación, para comprobar que los datos ingresados sean los correctos. (TF-30)</t>
   </si>
   <si>
-    <t>Como secretaria quiero guardar el filtro de la lista de forma periódica y que se imprima la lista automáticamente para así optimizar el tiempo de consultas reiterativas. (TF-15)</t>
-  </si>
-  <si>
     <t>Como secretaria quiero reagendar turnos para cuando un médico le surge una urgencia. (TF-10)</t>
   </si>
   <si>
-    <t>Como paciente quiero indicar un rango de fechas para visualizar los turnos y/o indicar el turno de preferencia (TF-24)</t>
-  </si>
-  <si>
-    <t>Como paciente quiero visualizar los turnos disponibles de acuerdo al filtro indicado para poder sacar un nuevo turno. (TF-1)</t>
-  </si>
-  <si>
     <t>Como paciente quiero recibir un email con el detalle del turno solicitado en la aplicación, para obtener un comprobante de dicho turno. (TF-3)</t>
+  </si>
+  <si>
+    <t>fin Release 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d-m"/>
+    <numFmt numFmtId="164" formatCode="d\-m"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font/>
     <font>
-      <sz val="11.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -244,43 +266,62 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
-    <border/>
+  <borders count="6">
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -290,101 +331,115 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -574,311 +629,363 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.88"/>
-    <col customWidth="1" min="2" max="2" width="16.75"/>
-    <col customWidth="1" min="3" max="3" width="14.0"/>
-    <col customWidth="1" min="4" max="4" width="27.38"/>
-    <col customWidth="1" min="5" max="5" width="25.13"/>
-    <col customWidth="1" min="6" max="6" width="3.63"/>
-    <col customWidth="1" min="7" max="7" width="17.0"/>
-    <col customWidth="1" min="8" max="8" width="17.25"/>
-    <col customWidth="1" min="9" max="9" width="19.38"/>
-    <col customWidth="1" min="10" max="10" width="20.13"/>
-    <col customWidth="1" min="11" max="11" width="5.0"/>
-    <col customWidth="1" min="12" max="12" width="17.5"/>
-    <col customWidth="1" min="13" max="13" width="13.0"/>
-    <col customWidth="1" min="14" max="14" width="3.63"/>
-    <col customWidth="1" min="15" max="15" width="16.88"/>
-    <col customWidth="1" min="16" max="16" width="23.25"/>
-    <col customWidth="1" min="17" max="17" width="18.5"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="5" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="3.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="23.28515625" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="7" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="7" t="s">
+      <c r="M2" s="22"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="5"/>
-    </row>
-    <row r="3" ht="20.25" customHeight="1"/>
-    <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="P2" s="22"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11" t="s">
+      <c r="E4" s="25"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11" t="s">
+      <c r="J4" s="25"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="11" t="s">
+      <c r="N4" s="4"/>
+      <c r="O4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" ht="40.5" customHeight="1">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="14" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="14" t="s">
+      <c r="K6" s="10"/>
+      <c r="L6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="19"/>
-      <c r="O6" s="14" t="s">
+      <c r="N6" s="12"/>
+      <c r="O6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Q6" s="16"/>
-    </row>
-    <row r="7">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-    </row>
-    <row r="8" ht="99.75" customHeight="1">
-      <c r="A8" s="20" t="s">
+      <c r="Q6" s="9"/>
+    </row>
+    <row r="7" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+    </row>
+    <row r="8" spans="1:17" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="K8" s="10"/>
+      <c r="L8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="21" t="s">
+      <c r="M8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="N8" s="10"/>
+      <c r="O8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N8" s="17"/>
-      <c r="O8" s="21" t="s">
+      <c r="P8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="Q8" s="9"/>
+    </row>
+    <row r="9" spans="1:17" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B9" s="9"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="Q8" s="16"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="16"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="21" t="s">
+      <c r="E9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="9"/>
+    </row>
+    <row r="10" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="21" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+    </row>
+    <row r="11" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+    </row>
+    <row r="12" spans="1:17" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="16"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="21" t="s">
+      <c r="I12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="J12" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="21" t="s">
+      <c r="K12" s="9"/>
+      <c r="M12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="21" t="s">
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:17" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="D13" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="21" t="s">
+      <c r="H13" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-    </row>
-    <row r="12">
-      <c r="D12" s="21" t="s">
+      <c r="J13" s="14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13">
-      <c r="D13" s="21" t="s">
+    <row r="14" spans="1:17" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="D14" s="14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="25"/>
-      <c r="B17" s="26"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
+      <c r="J14" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="D15" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+    </row>
+    <row r="17" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+    </row>
+    <row r="18" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+    </row>
+    <row r="19" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+    </row>
+    <row r="20" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A11:P11"/>
+    <mergeCell ref="A16:P16"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="L2:M2"/>
@@ -887,6 +994,6 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="I4:J4"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>